<commit_message>
Tyron - Report Column Formatting
</commit_message>
<xml_diff>
--- a/UDM.Insurance.Interface/Templates/ReportTemplateBatchReport.xlsx
+++ b/UDM.Insurance.Interface/Templates/ReportTemplateBatchReport.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kyleh\source\repos\Insure20230223\UDM.Insurance.Interface\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4F1E14E-2FA8-4160-8054-5D6DB7A11396}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE1AD030-0D11-41FF-9B77-79A595ACD735}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-23490" yWindow="2040" windowWidth="23250" windowHeight="10995" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1053,7 +1053,7 @@
     <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="199">
+  <cellXfs count="198">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1606,9 +1606,6 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="20% - Accent1" xfId="4" builtinId="30"/>
@@ -7121,7 +7118,7 @@
   <dimension ref="A1:AA26"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" topLeftCell="C4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="R8" sqref="R8"/>
+      <selection activeCell="O8" sqref="O8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="1.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7323,7 +7320,6 @@
       <c r="H8" s="3"/>
       <c r="K8" s="118"/>
       <c r="L8" s="118"/>
-      <c r="O8" s="198"/>
       <c r="R8" s="118"/>
       <c r="S8" s="3"/>
       <c r="V8" s="118"/>
@@ -7349,7 +7345,7 @@
       <c r="L9" s="119"/>
       <c r="M9" s="10"/>
       <c r="N9" s="10"/>
-      <c r="O9" s="162"/>
+      <c r="O9" s="11"/>
       <c r="P9" s="10"/>
       <c r="Q9" s="10"/>
       <c r="R9" s="119"/>
@@ -7384,7 +7380,7 @@
       <c r="L10" s="119"/>
       <c r="M10" s="10"/>
       <c r="N10" s="10"/>
-      <c r="O10" s="162"/>
+      <c r="O10" s="11"/>
       <c r="P10" s="10"/>
       <c r="Q10" s="10"/>
       <c r="R10" s="119"/>

</xml_diff>

<commit_message>
Tyron - Report Template Formatting
</commit_message>
<xml_diff>
--- a/UDM.Insurance.Interface/Templates/ReportTemplateBatchReport.xlsx
+++ b/UDM.Insurance.Interface/Templates/ReportTemplateBatchReport.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kyleh\source\repos\Insure20230223\UDM.Insurance.Interface\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE1AD030-0D11-41FF-9B77-79A595ACD735}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B137734-78BC-4C1F-9E23-87FEB2D910B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23490" yWindow="2040" windowWidth="23250" windowHeight="10995" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Default (Old)" sheetId="13" r:id="rId1"/>
@@ -7118,7 +7118,7 @@
   <dimension ref="A1:AA26"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" topLeftCell="C4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O8" sqref="O8"/>
+      <selection activeCell="O8" sqref="O8:O10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="1.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7320,6 +7320,7 @@
       <c r="H8" s="3"/>
       <c r="K8" s="118"/>
       <c r="L8" s="118"/>
+      <c r="O8" s="118"/>
       <c r="R8" s="118"/>
       <c r="S8" s="3"/>
       <c r="V8" s="118"/>
@@ -7345,7 +7346,7 @@
       <c r="L9" s="119"/>
       <c r="M9" s="10"/>
       <c r="N9" s="10"/>
-      <c r="O9" s="11"/>
+      <c r="O9" s="119"/>
       <c r="P9" s="10"/>
       <c r="Q9" s="10"/>
       <c r="R9" s="119"/>
@@ -7380,7 +7381,7 @@
       <c r="L10" s="119"/>
       <c r="M10" s="10"/>
       <c r="N10" s="10"/>
-      <c r="O10" s="11"/>
+      <c r="O10" s="119"/>
       <c r="P10" s="10"/>
       <c r="Q10" s="10"/>
       <c r="R10" s="119"/>

</xml_diff>

<commit_message>
Tyron Column formatting Changes
</commit_message>
<xml_diff>
--- a/UDM.Insurance.Interface/Templates/ReportTemplateBatchReport.xlsx
+++ b/UDM.Insurance.Interface/Templates/ReportTemplateBatchReport.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kyleh\source\repos\Insure20230223\UDM.Insurance.Interface\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B137734-78BC-4C1F-9E23-87FEB2D910B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01FA7699-BBF0-433D-BF73-905CE2CEE0C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -325,7 +325,7 @@
     <numFmt numFmtId="166" formatCode="&quot;R&quot;\ #,##0"/>
     <numFmt numFmtId="167" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -476,6 +476,21 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1053,7 +1068,7 @@
     <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="198">
+  <cellXfs count="222">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1606,6 +1621,76 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="22" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="22" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="22" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="21" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="21" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="21" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="21" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="20% - Accent1" xfId="4" builtinId="30"/>
@@ -7118,1088 +7203,1089 @@
   <dimension ref="A1:AA26"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" topLeftCell="C4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O8" sqref="O8:O10"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="1.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="1.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.85546875" style="3" hidden="1" customWidth="1"/>
-    <col min="2" max="2" width="12.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.5703125" style="8" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="11.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.42578125" style="5" customWidth="1"/>
-    <col min="9" max="9" width="8.140625" style="3" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="12.5703125" style="3" customWidth="1"/>
-    <col min="11" max="12" width="11.140625" style="5" customWidth="1"/>
-    <col min="13" max="13" width="8.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10" style="3" customWidth="1"/>
-    <col min="15" max="15" width="10.85546875" style="5" customWidth="1"/>
-    <col min="16" max="16" width="8.85546875" style="3" customWidth="1"/>
-    <col min="17" max="17" width="10" style="3" hidden="1" customWidth="1"/>
-    <col min="18" max="18" width="8.28515625" style="3" customWidth="1"/>
-    <col min="19" max="19" width="3.28515625" style="5" hidden="1" customWidth="1"/>
-    <col min="20" max="20" width="9.7109375" style="3" hidden="1" customWidth="1"/>
-    <col min="21" max="21" width="10.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="10.7109375" style="3" customWidth="1"/>
-    <col min="23" max="23" width="9.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="15" style="3" customWidth="1"/>
-    <col min="25" max="25" width="11.42578125" style="3" customWidth="1"/>
-    <col min="26" max="26" width="11.42578125" style="3" hidden="1" customWidth="1"/>
-    <col min="27" max="27" width="32.5703125" customWidth="1"/>
+    <col min="1" max="1" width="23.85546875" style="202" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" style="202" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.140625" style="202" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" style="202" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.5703125" style="203" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="11.5703125" style="203" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.140625" style="202" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.42578125" style="204" customWidth="1"/>
+    <col min="9" max="9" width="8.140625" style="202" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="12.5703125" style="202" customWidth="1"/>
+    <col min="11" max="12" width="11.140625" style="204" customWidth="1"/>
+    <col min="13" max="13" width="9" style="202" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10" style="202" customWidth="1"/>
+    <col min="15" max="15" width="10.85546875" style="204" customWidth="1"/>
+    <col min="16" max="16" width="8.85546875" style="202" customWidth="1"/>
+    <col min="17" max="17" width="10" style="202" hidden="1" customWidth="1"/>
+    <col min="18" max="18" width="8.28515625" style="202" customWidth="1"/>
+    <col min="19" max="19" width="3.28515625" style="204" hidden="1" customWidth="1"/>
+    <col min="20" max="20" width="9.7109375" style="202" hidden="1" customWidth="1"/>
+    <col min="21" max="21" width="10.7109375" style="202" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="10.7109375" style="202" customWidth="1"/>
+    <col min="23" max="23" width="9.5703125" style="202" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="15" style="202" customWidth="1"/>
+    <col min="25" max="25" width="11.42578125" style="202" customWidth="1"/>
+    <col min="26" max="26" width="11.42578125" style="202" hidden="1" customWidth="1"/>
+    <col min="27" max="27" width="32.5703125" style="201" customWidth="1"/>
+    <col min="28" max="16384" width="1.140625" style="201"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="27.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="175" t="s">
+    <row r="1" spans="1:27" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="198" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="176"/>
-      <c r="C1" s="176"/>
-      <c r="D1" s="176"/>
-      <c r="E1" s="176"/>
-      <c r="F1" s="176"/>
-      <c r="G1" s="176"/>
-      <c r="H1" s="176"/>
-      <c r="I1" s="176"/>
-      <c r="J1" s="176"/>
-      <c r="K1" s="176"/>
-      <c r="L1" s="176"/>
-      <c r="M1" s="176"/>
-      <c r="N1" s="176"/>
-      <c r="O1" s="176"/>
-      <c r="P1" s="176"/>
-      <c r="Q1" s="176"/>
-      <c r="R1" s="176"/>
-      <c r="S1" s="176"/>
-      <c r="T1" s="176"/>
-      <c r="U1" s="176"/>
-      <c r="V1" s="176"/>
-      <c r="W1" s="176"/>
-      <c r="X1" s="176"/>
-      <c r="Y1" s="176"/>
-      <c r="Z1" s="176"/>
-      <c r="AA1" s="177"/>
-    </row>
-    <row r="2" spans="1:27" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:27" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A3" s="172" t="s">
+      <c r="B1" s="199"/>
+      <c r="C1" s="199"/>
+      <c r="D1" s="199"/>
+      <c r="E1" s="199"/>
+      <c r="F1" s="199"/>
+      <c r="G1" s="199"/>
+      <c r="H1" s="199"/>
+      <c r="I1" s="199"/>
+      <c r="J1" s="199"/>
+      <c r="K1" s="199"/>
+      <c r="L1" s="199"/>
+      <c r="M1" s="199"/>
+      <c r="N1" s="199"/>
+      <c r="O1" s="199"/>
+      <c r="P1" s="199"/>
+      <c r="Q1" s="199"/>
+      <c r="R1" s="199"/>
+      <c r="S1" s="199"/>
+      <c r="T1" s="199"/>
+      <c r="U1" s="199"/>
+      <c r="V1" s="199"/>
+      <c r="W1" s="199"/>
+      <c r="X1" s="199"/>
+      <c r="Y1" s="199"/>
+      <c r="Z1" s="199"/>
+      <c r="AA1" s="200"/>
+    </row>
+    <row r="2" spans="1:27" ht="16.5" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A3" s="205" t="s">
         <v>32</v>
       </c>
-      <c r="B3" s="172"/>
-      <c r="C3" s="172"/>
-      <c r="D3" s="172"/>
-      <c r="E3" s="172"/>
-      <c r="F3" s="172"/>
-      <c r="G3" s="172"/>
-      <c r="H3" s="172"/>
-      <c r="I3" s="172"/>
-      <c r="J3" s="172"/>
-      <c r="K3" s="172"/>
-      <c r="L3" s="172"/>
-      <c r="M3" s="172"/>
-      <c r="N3" s="172"/>
-      <c r="O3" s="172"/>
-      <c r="P3" s="172"/>
-      <c r="Q3" s="172"/>
-      <c r="R3" s="172"/>
-      <c r="S3" s="172"/>
-      <c r="T3" s="172"/>
-      <c r="U3" s="172"/>
-      <c r="V3" s="172"/>
-      <c r="W3" s="172"/>
-      <c r="X3" s="172"/>
-      <c r="Y3" s="172"/>
-      <c r="Z3" s="172"/>
-      <c r="AA3" s="172"/>
+      <c r="B3" s="205"/>
+      <c r="C3" s="205"/>
+      <c r="D3" s="205"/>
+      <c r="E3" s="205"/>
+      <c r="F3" s="205"/>
+      <c r="G3" s="205"/>
+      <c r="H3" s="205"/>
+      <c r="I3" s="205"/>
+      <c r="J3" s="205"/>
+      <c r="K3" s="205"/>
+      <c r="L3" s="205"/>
+      <c r="M3" s="205"/>
+      <c r="N3" s="205"/>
+      <c r="O3" s="205"/>
+      <c r="P3" s="205"/>
+      <c r="Q3" s="205"/>
+      <c r="R3" s="205"/>
+      <c r="S3" s="205"/>
+      <c r="T3" s="205"/>
+      <c r="U3" s="205"/>
+      <c r="V3" s="205"/>
+      <c r="W3" s="205"/>
+      <c r="X3" s="205"/>
+      <c r="Y3" s="205"/>
+      <c r="Z3" s="205"/>
+      <c r="AA3" s="205"/>
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="V4" s="174" t="s">
+      <c r="V4" s="206" t="s">
         <v>31</v>
       </c>
-      <c r="W4" s="174"/>
-      <c r="X4" s="174"/>
-      <c r="Y4" s="174"/>
-      <c r="Z4" s="174"/>
+      <c r="W4" s="206"/>
+      <c r="X4" s="206"/>
+      <c r="Y4" s="206"/>
+      <c r="Z4" s="206"/>
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="V5" s="174" t="s">
+      <c r="V5" s="206" t="s">
         <v>78</v>
       </c>
-      <c r="W5" s="174"/>
-      <c r="X5" s="174"/>
-      <c r="Y5" s="174"/>
-      <c r="Z5" s="174"/>
+      <c r="W5" s="206"/>
+      <c r="X5" s="206"/>
+      <c r="Y5" s="206"/>
+      <c r="Z5" s="206"/>
     </row>
     <row r="7" spans="1:27" ht="62.85" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="207" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="208" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="208" t="s">
         <v>2</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D7" s="208" t="s">
         <v>3</v>
       </c>
-      <c r="E7" s="7" t="s">
+      <c r="E7" s="209" t="s">
         <v>4</v>
       </c>
-      <c r="F7" s="7" t="s">
+      <c r="F7" s="209" t="s">
         <v>5</v>
       </c>
-      <c r="G7" s="4" t="s">
+      <c r="G7" s="210" t="s">
         <v>7</v>
       </c>
-      <c r="H7" s="2" t="s">
+      <c r="H7" s="207" t="s">
         <v>6</v>
       </c>
-      <c r="I7" s="1" t="s">
+      <c r="I7" s="208" t="s">
         <v>8</v>
       </c>
-      <c r="J7" s="1" t="s">
+      <c r="J7" s="208" t="s">
         <v>79</v>
       </c>
-      <c r="K7" s="6" t="s">
+      <c r="K7" s="211" t="s">
         <v>90</v>
       </c>
-      <c r="L7" s="6" t="s">
+      <c r="L7" s="211" t="s">
         <v>91</v>
       </c>
-      <c r="M7" s="1" t="s">
+      <c r="M7" s="208" t="s">
         <v>14</v>
       </c>
-      <c r="N7" s="1" t="s">
+      <c r="N7" s="208" t="s">
         <v>9</v>
       </c>
-      <c r="O7" s="6" t="s">
+      <c r="O7" s="211" t="s">
         <v>10</v>
       </c>
-      <c r="P7" s="1" t="s">
+      <c r="P7" s="208" t="s">
         <v>11</v>
       </c>
-      <c r="Q7" s="1" t="s">
+      <c r="Q7" s="208" t="s">
         <v>12</v>
       </c>
-      <c r="R7" s="6" t="s">
+      <c r="R7" s="211" t="s">
         <v>13</v>
       </c>
-      <c r="S7" s="1" t="s">
+      <c r="S7" s="208" t="s">
         <v>18</v>
       </c>
-      <c r="T7" s="1" t="s">
+      <c r="T7" s="208" t="s">
         <v>21</v>
       </c>
-      <c r="U7" s="1" t="s">
+      <c r="U7" s="208" t="s">
         <v>70</v>
       </c>
-      <c r="V7" s="1" t="s">
+      <c r="V7" s="208" t="s">
         <v>71</v>
       </c>
-      <c r="W7" s="1" t="s">
+      <c r="W7" s="208" t="s">
         <v>66</v>
       </c>
-      <c r="X7" s="1" t="s">
+      <c r="X7" s="208" t="s">
         <v>69</v>
       </c>
-      <c r="Y7" s="2" t="s">
+      <c r="Y7" s="207" t="s">
         <v>16</v>
       </c>
-      <c r="Z7" s="1" t="s">
+      <c r="Z7" s="208" t="s">
         <v>67</v>
       </c>
-      <c r="AA7" s="2" t="s">
+      <c r="AA7" s="207" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="G8" s="118"/>
-      <c r="H8" s="3"/>
-      <c r="K8" s="118"/>
-      <c r="L8" s="118"/>
-      <c r="O8" s="118"/>
-      <c r="R8" s="118"/>
-      <c r="S8" s="3"/>
-      <c r="V8" s="118"/>
-      <c r="Y8" s="8"/>
-      <c r="AA8" s="3"/>
+      <c r="G8" s="212"/>
+      <c r="H8" s="202"/>
+      <c r="K8" s="212"/>
+      <c r="L8" s="212"/>
+      <c r="O8" s="212"/>
+      <c r="R8" s="212"/>
+      <c r="S8" s="202"/>
+      <c r="V8" s="212"/>
+      <c r="Y8" s="203"/>
+      <c r="AA8" s="202"/>
     </row>
     <row r="9" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A9" s="13" t="s">
+      <c r="A9" s="213" t="s">
         <v>29</v>
       </c>
-      <c r="B9" s="173" t="s">
+      <c r="B9" s="214" t="s">
         <v>29</v>
       </c>
-      <c r="C9" s="173"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="12"/>
-      <c r="G9" s="119"/>
-      <c r="H9" s="10"/>
-      <c r="I9" s="10"/>
-      <c r="J9" s="10"/>
-      <c r="K9" s="119"/>
-      <c r="L9" s="119"/>
-      <c r="M9" s="10"/>
-      <c r="N9" s="10"/>
-      <c r="O9" s="119"/>
-      <c r="P9" s="10"/>
-      <c r="Q9" s="10"/>
-      <c r="R9" s="119"/>
-      <c r="S9" s="10"/>
-      <c r="T9" s="10"/>
-      <c r="U9" s="10"/>
-      <c r="V9" s="119"/>
-      <c r="W9" s="10"/>
-      <c r="X9" s="10"/>
-      <c r="Y9" s="10" t="s">
+      <c r="C9" s="214"/>
+      <c r="D9" s="215"/>
+      <c r="E9" s="216"/>
+      <c r="F9" s="216"/>
+      <c r="G9" s="217"/>
+      <c r="H9" s="215"/>
+      <c r="I9" s="215"/>
+      <c r="J9" s="215"/>
+      <c r="K9" s="217"/>
+      <c r="L9" s="217"/>
+      <c r="M9" s="215"/>
+      <c r="N9" s="215"/>
+      <c r="O9" s="217"/>
+      <c r="P9" s="215"/>
+      <c r="Q9" s="215"/>
+      <c r="R9" s="217"/>
+      <c r="S9" s="215"/>
+      <c r="T9" s="215"/>
+      <c r="U9" s="215"/>
+      <c r="V9" s="217"/>
+      <c r="W9" s="215"/>
+      <c r="X9" s="215"/>
+      <c r="Y9" s="215" t="s">
         <v>22</v>
       </c>
-      <c r="Z9" s="9"/>
-      <c r="AA9" s="9"/>
+      <c r="Z9" s="218"/>
+      <c r="AA9" s="218"/>
     </row>
     <row r="10" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A10" s="13" t="s">
+      <c r="A10" s="213" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="173" t="s">
+      <c r="B10" s="214" t="s">
         <v>23</v>
       </c>
-      <c r="C10" s="173"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="119"/>
-      <c r="H10" s="10"/>
-      <c r="I10" s="10"/>
-      <c r="J10" s="10"/>
-      <c r="K10" s="119"/>
-      <c r="L10" s="119"/>
-      <c r="M10" s="10"/>
-      <c r="N10" s="10"/>
-      <c r="O10" s="119"/>
-      <c r="P10" s="10"/>
-      <c r="Q10" s="10"/>
-      <c r="R10" s="119"/>
-      <c r="S10" s="10"/>
-      <c r="T10" s="10"/>
-      <c r="U10" s="10"/>
-      <c r="V10" s="119"/>
-      <c r="W10" s="10"/>
-      <c r="X10" s="10"/>
-      <c r="Y10" s="10" t="s">
+      <c r="C10" s="214"/>
+      <c r="D10" s="215"/>
+      <c r="E10" s="216"/>
+      <c r="F10" s="216"/>
+      <c r="G10" s="217"/>
+      <c r="H10" s="215"/>
+      <c r="I10" s="215"/>
+      <c r="J10" s="215"/>
+      <c r="K10" s="217"/>
+      <c r="L10" s="217"/>
+      <c r="M10" s="215"/>
+      <c r="N10" s="215"/>
+      <c r="O10" s="217"/>
+      <c r="P10" s="215"/>
+      <c r="Q10" s="215"/>
+      <c r="R10" s="217"/>
+      <c r="S10" s="215"/>
+      <c r="T10" s="215"/>
+      <c r="U10" s="215"/>
+      <c r="V10" s="217"/>
+      <c r="W10" s="215"/>
+      <c r="X10" s="215"/>
+      <c r="Y10" s="215" t="s">
         <v>22</v>
       </c>
-      <c r="Z10" s="9"/>
-      <c r="AA10" s="9"/>
+      <c r="Z10" s="218"/>
+      <c r="AA10" s="218"/>
     </row>
     <row r="11" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="X11" s="5"/>
-    </row>
-    <row r="12" spans="1:27" ht="60" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
+      <c r="X11" s="204"/>
+    </row>
+    <row r="12" spans="1:27" ht="63" x14ac:dyDescent="0.25">
+      <c r="A12" s="207" t="s">
         <v>0</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="208" t="s">
         <v>1</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C12" s="208" t="s">
         <v>2</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="D12" s="208" t="s">
         <v>3</v>
       </c>
-      <c r="E12" s="7" t="s">
+      <c r="E12" s="209" t="s">
         <v>4</v>
       </c>
-      <c r="F12" s="7" t="s">
+      <c r="F12" s="209" t="s">
         <v>5</v>
       </c>
-      <c r="G12" s="2" t="s">
+      <c r="G12" s="207" t="s">
         <v>6</v>
       </c>
-      <c r="H12" s="4" t="s">
+      <c r="H12" s="210" t="s">
         <v>7</v>
       </c>
-      <c r="I12" s="1" t="s">
+      <c r="I12" s="208" t="s">
         <v>8</v>
       </c>
-      <c r="J12" s="1" t="s">
+      <c r="J12" s="208" t="s">
         <v>9</v>
       </c>
-      <c r="K12" s="6" t="s">
+      <c r="K12" s="211" t="s">
         <v>10</v>
       </c>
-      <c r="L12" s="1" t="s">
+      <c r="L12" s="208" t="s">
         <v>11</v>
       </c>
-      <c r="M12" s="1" t="s">
+      <c r="M12" s="208" t="s">
         <v>12</v>
       </c>
-      <c r="N12" s="6" t="s">
+      <c r="N12" s="211" t="s">
         <v>13</v>
       </c>
-      <c r="O12" s="1" t="s">
+      <c r="O12" s="208" t="s">
         <v>14</v>
       </c>
-      <c r="P12" s="1" t="s">
+      <c r="P12" s="208" t="s">
         <v>18</v>
       </c>
-      <c r="Q12" s="1" t="s">
+      <c r="Q12" s="208" t="s">
         <v>21</v>
       </c>
-      <c r="R12" s="6" t="s">
+      <c r="R12" s="211" t="s">
         <v>15</v>
       </c>
-      <c r="S12" s="1" t="s">
+      <c r="S12" s="208" t="s">
         <v>66</v>
       </c>
-      <c r="T12" s="2" t="s">
+      <c r="T12" s="207" t="s">
         <v>16</v>
       </c>
-      <c r="U12" s="1" t="s">
+      <c r="U12" s="208" t="s">
         <v>69</v>
       </c>
-      <c r="V12" s="1" t="s">
+      <c r="V12" s="208" t="s">
         <v>70</v>
       </c>
-      <c r="W12" s="6" t="s">
+      <c r="W12" s="211" t="s">
         <v>71</v>
       </c>
-      <c r="X12" s="1" t="s">
+      <c r="X12" s="208" t="s">
         <v>67</v>
       </c>
-      <c r="Y12" s="2" t="s">
+      <c r="Y12" s="207" t="s">
         <v>17</v>
       </c>
-      <c r="Z12"/>
+      <c r="Z12" s="201"/>
     </row>
     <row r="13" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
+      <c r="A13" s="202" t="s">
         <v>28</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="202" t="s">
         <v>27</v>
       </c>
-      <c r="C13" s="3">
+      <c r="C13" s="202">
         <v>47</v>
       </c>
-      <c r="D13" s="3">
+      <c r="D13" s="202">
         <v>43</v>
       </c>
-      <c r="E13" s="8">
+      <c r="E13" s="203">
         <v>42158</v>
       </c>
-      <c r="F13" s="8">
+      <c r="F13" s="203">
         <v>42249</v>
       </c>
-      <c r="G13" s="3">
+      <c r="G13" s="202">
         <v>1571</v>
       </c>
-      <c r="H13" s="5">
+      <c r="H13" s="204">
         <v>0.26500000000000001</v>
       </c>
-      <c r="I13" s="3">
+      <c r="I13" s="202">
         <v>416.3</v>
       </c>
-      <c r="J13" s="3">
+      <c r="J13" s="202">
         <v>396</v>
       </c>
-      <c r="K13" s="158">
+      <c r="K13" s="219">
         <v>0.25206874602163998</v>
       </c>
-      <c r="L13" s="3">
+      <c r="L13" s="202">
         <v>20</v>
       </c>
-      <c r="M13" s="3">
+      <c r="M13" s="202">
         <v>765</v>
       </c>
-      <c r="N13" s="5">
+      <c r="N13" s="204">
         <v>0.48695098663271003</v>
       </c>
-      <c r="O13" s="3">
+      <c r="O13" s="202">
         <v>237</v>
       </c>
-      <c r="P13" s="3">
+      <c r="P13" s="202">
         <v>160</v>
       </c>
-      <c r="Q13" s="3">
+      <c r="Q13" s="202">
         <v>0</v>
       </c>
-      <c r="R13" s="5">
+      <c r="R13" s="204">
         <v>0.84086569064289995</v>
       </c>
-      <c r="S13" s="3"/>
-      <c r="T13" s="3" t="s">
+      <c r="S13" s="202"/>
+      <c r="T13" s="202" t="s">
         <v>26</v>
       </c>
-      <c r="W13" s="5"/>
-      <c r="Y13" s="3" t="s">
+      <c r="W13" s="204"/>
+      <c r="Y13" s="202" t="s">
         <v>25</v>
       </c>
-      <c r="Z13"/>
+      <c r="Z13" s="201"/>
     </row>
     <row r="14" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="202" t="s">
         <v>28</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="202" t="s">
         <v>27</v>
       </c>
-      <c r="C14" s="3">
+      <c r="C14" s="202">
         <v>47</v>
       </c>
-      <c r="D14" s="3">
+      <c r="D14" s="202">
         <v>43</v>
       </c>
-      <c r="E14" s="8">
+      <c r="E14" s="203">
         <v>42158</v>
       </c>
-      <c r="F14" s="8">
+      <c r="F14" s="203">
         <v>42249</v>
       </c>
-      <c r="G14" s="3">
+      <c r="G14" s="202">
         <v>1571</v>
       </c>
-      <c r="H14" s="5">
+      <c r="H14" s="204">
         <v>0.26500000000000001</v>
       </c>
-      <c r="I14" s="3">
+      <c r="I14" s="202">
         <v>416.3</v>
       </c>
-      <c r="J14" s="3">
+      <c r="J14" s="202">
         <v>396</v>
       </c>
-      <c r="K14" s="158">
+      <c r="K14" s="219">
         <v>0.25206874602163998</v>
       </c>
-      <c r="L14" s="3">
+      <c r="L14" s="202">
         <v>20</v>
       </c>
-      <c r="M14" s="3">
+      <c r="M14" s="202">
         <v>765</v>
       </c>
-      <c r="N14" s="5">
+      <c r="N14" s="204">
         <v>0.48695098663271003</v>
       </c>
-      <c r="O14" s="3">
+      <c r="O14" s="202">
         <v>237</v>
       </c>
-      <c r="P14" s="3">
+      <c r="P14" s="202">
         <v>160</v>
       </c>
-      <c r="Q14" s="3">
+      <c r="Q14" s="202">
         <v>0</v>
       </c>
-      <c r="R14" s="5">
+      <c r="R14" s="204">
         <v>0.84086569064289995</v>
       </c>
-      <c r="S14" s="3"/>
-      <c r="T14" s="3" t="s">
+      <c r="S14" s="202"/>
+      <c r="T14" s="202" t="s">
         <v>26</v>
       </c>
-      <c r="W14" s="5"/>
-      <c r="Y14" s="3" t="s">
+      <c r="W14" s="204"/>
+      <c r="Y14" s="202" t="s">
         <v>25</v>
       </c>
-      <c r="Z14"/>
+      <c r="Z14" s="201"/>
     </row>
     <row r="15" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A15" s="10" t="s">
+      <c r="A15" s="215" t="s">
         <v>24</v>
       </c>
-      <c r="B15" s="10"/>
-      <c r="C15" s="10"/>
-      <c r="D15" s="10"/>
-      <c r="E15" s="12"/>
-      <c r="F15" s="12"/>
-      <c r="G15" s="10">
+      <c r="B15" s="215"/>
+      <c r="C15" s="215"/>
+      <c r="D15" s="215"/>
+      <c r="E15" s="216"/>
+      <c r="F15" s="216"/>
+      <c r="G15" s="215">
         <v>1571</v>
       </c>
-      <c r="H15" s="11"/>
-      <c r="I15" s="10">
+      <c r="H15" s="220"/>
+      <c r="I15" s="215">
         <v>416.3</v>
       </c>
-      <c r="J15" s="10">
+      <c r="J15" s="215">
         <v>396</v>
       </c>
-      <c r="K15" s="159">
+      <c r="K15" s="221">
         <v>0.25206874602163998</v>
       </c>
-      <c r="L15" s="10">
+      <c r="L15" s="215">
         <v>20</v>
       </c>
-      <c r="M15" s="10">
+      <c r="M15" s="215">
         <v>765</v>
       </c>
-      <c r="N15" s="11">
+      <c r="N15" s="220">
         <v>0.48695098663271003</v>
       </c>
-      <c r="O15" s="10">
+      <c r="O15" s="215">
         <v>237</v>
       </c>
-      <c r="P15" s="10">
+      <c r="P15" s="215">
         <v>160</v>
       </c>
-      <c r="Q15" s="10">
+      <c r="Q15" s="215">
         <v>0</v>
       </c>
-      <c r="R15" s="11">
+      <c r="R15" s="220">
         <v>0.84086569064289995</v>
       </c>
-      <c r="S15" s="10"/>
-      <c r="T15" s="10" t="s">
+      <c r="S15" s="215"/>
+      <c r="T15" s="215" t="s">
         <v>22</v>
       </c>
-      <c r="U15" s="10"/>
-      <c r="V15" s="10"/>
-      <c r="W15" s="11"/>
-      <c r="X15" s="9"/>
-      <c r="Y15" s="9"/>
-      <c r="Z15"/>
+      <c r="U15" s="215"/>
+      <c r="V15" s="215"/>
+      <c r="W15" s="220"/>
+      <c r="X15" s="218"/>
+      <c r="Y15" s="218"/>
+      <c r="Z15" s="201"/>
     </row>
     <row r="16" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A16" s="13" t="s">
+      <c r="A16" s="213" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="10"/>
-      <c r="C16" s="10"/>
-      <c r="D16" s="10"/>
-      <c r="E16" s="12"/>
-      <c r="F16" s="12"/>
-      <c r="G16" s="10">
+      <c r="B16" s="215"/>
+      <c r="C16" s="215"/>
+      <c r="D16" s="215"/>
+      <c r="E16" s="216"/>
+      <c r="F16" s="216"/>
+      <c r="G16" s="215">
         <v>1571</v>
       </c>
-      <c r="H16" s="11"/>
-      <c r="I16" s="10">
+      <c r="H16" s="220"/>
+      <c r="I16" s="215">
         <v>416.3</v>
       </c>
-      <c r="J16" s="10">
+      <c r="J16" s="215">
         <v>396</v>
       </c>
-      <c r="K16" s="159">
+      <c r="K16" s="221">
         <v>0.25206874602163998</v>
       </c>
-      <c r="L16" s="10">
+      <c r="L16" s="215">
         <v>20</v>
       </c>
-      <c r="M16" s="10">
+      <c r="M16" s="215">
         <v>765</v>
       </c>
-      <c r="N16" s="11">
+      <c r="N16" s="220">
         <v>0.48695098663271003</v>
       </c>
-      <c r="O16" s="10">
+      <c r="O16" s="215">
         <v>237</v>
       </c>
-      <c r="P16" s="10">
+      <c r="P16" s="215">
         <v>160</v>
       </c>
-      <c r="Q16" s="10">
+      <c r="Q16" s="215">
         <v>0</v>
       </c>
-      <c r="R16" s="11">
+      <c r="R16" s="220">
         <v>0.84086569064289995</v>
       </c>
-      <c r="S16" s="10"/>
-      <c r="T16" s="10" t="s">
+      <c r="S16" s="215"/>
+      <c r="T16" s="215" t="s">
         <v>22</v>
       </c>
-      <c r="U16" s="10"/>
-      <c r="V16" s="10"/>
-      <c r="W16" s="11"/>
-      <c r="X16" s="9"/>
-      <c r="Y16" s="9"/>
-      <c r="Z16"/>
+      <c r="U16" s="215"/>
+      <c r="V16" s="215"/>
+      <c r="W16" s="220"/>
+      <c r="X16" s="218"/>
+      <c r="Y16" s="218"/>
+      <c r="Z16" s="201"/>
     </row>
     <row r="17" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="L17" s="3"/>
-      <c r="N17" s="5"/>
-      <c r="O17" s="3"/>
-      <c r="R17" s="5"/>
-      <c r="S17" s="3"/>
-      <c r="W17" s="5"/>
-      <c r="Z17"/>
-    </row>
-    <row r="18" spans="1:26" ht="60" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
+      <c r="L17" s="202"/>
+      <c r="N17" s="204"/>
+      <c r="O17" s="202"/>
+      <c r="R17" s="204"/>
+      <c r="S17" s="202"/>
+      <c r="W17" s="204"/>
+      <c r="Z17" s="201"/>
+    </row>
+    <row r="18" spans="1:26" ht="63" x14ac:dyDescent="0.25">
+      <c r="A18" s="207" t="s">
         <v>0</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" s="208" t="s">
         <v>1</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="C18" s="208" t="s">
         <v>2</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="D18" s="208" t="s">
         <v>3</v>
       </c>
-      <c r="E18" s="7" t="s">
+      <c r="E18" s="209" t="s">
         <v>4</v>
       </c>
-      <c r="F18" s="7" t="s">
+      <c r="F18" s="209" t="s">
         <v>5</v>
       </c>
-      <c r="G18" s="2" t="s">
+      <c r="G18" s="207" t="s">
         <v>6</v>
       </c>
-      <c r="H18" s="4" t="s">
+      <c r="H18" s="210" t="s">
         <v>7</v>
       </c>
-      <c r="I18" s="1" t="s">
+      <c r="I18" s="208" t="s">
         <v>8</v>
       </c>
-      <c r="J18" s="1" t="s">
+      <c r="J18" s="208" t="s">
         <v>9</v>
       </c>
-      <c r="K18" s="6" t="s">
+      <c r="K18" s="211" t="s">
         <v>10</v>
       </c>
-      <c r="L18" s="1" t="s">
+      <c r="L18" s="208" t="s">
         <v>11</v>
       </c>
-      <c r="M18" s="1" t="s">
+      <c r="M18" s="208" t="s">
         <v>12</v>
       </c>
-      <c r="N18" s="6" t="s">
+      <c r="N18" s="211" t="s">
         <v>13</v>
       </c>
-      <c r="O18" s="1" t="s">
+      <c r="O18" s="208" t="s">
         <v>14</v>
       </c>
-      <c r="P18" s="1" t="s">
+      <c r="P18" s="208" t="s">
         <v>18</v>
       </c>
-      <c r="Q18" s="1" t="s">
+      <c r="Q18" s="208" t="s">
         <v>21</v>
       </c>
-      <c r="R18" s="6" t="s">
+      <c r="R18" s="211" t="s">
         <v>15</v>
       </c>
-      <c r="S18" s="1" t="s">
+      <c r="S18" s="208" t="s">
         <v>66</v>
       </c>
-      <c r="T18" s="2" t="s">
+      <c r="T18" s="207" t="s">
         <v>16</v>
       </c>
-      <c r="U18" s="1" t="s">
+      <c r="U18" s="208" t="s">
         <v>69</v>
       </c>
-      <c r="V18" s="1" t="s">
+      <c r="V18" s="208" t="s">
         <v>70</v>
       </c>
-      <c r="W18" s="6" t="s">
+      <c r="W18" s="211" t="s">
         <v>71</v>
       </c>
-      <c r="X18" s="1" t="s">
+      <c r="X18" s="208" t="s">
         <v>67</v>
       </c>
-      <c r="Y18" s="2" t="s">
+      <c r="Y18" s="207" t="s">
         <v>17</v>
       </c>
-      <c r="Z18"/>
+      <c r="Z18" s="201"/>
     </row>
     <row r="19" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
+      <c r="A19" s="202" t="s">
         <v>28</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="B19" s="202" t="s">
         <v>27</v>
       </c>
-      <c r="C19" s="3">
+      <c r="C19" s="202">
         <v>47</v>
       </c>
-      <c r="D19" s="3">
+      <c r="D19" s="202">
         <v>43</v>
       </c>
-      <c r="E19" s="8">
+      <c r="E19" s="203">
         <v>42158</v>
       </c>
-      <c r="F19" s="8">
+      <c r="F19" s="203">
         <v>42249</v>
       </c>
-      <c r="G19" s="3">
+      <c r="G19" s="202">
         <v>1571</v>
       </c>
-      <c r="H19" s="5">
+      <c r="H19" s="204">
         <v>0.26500000000000001</v>
       </c>
-      <c r="I19" s="3">
+      <c r="I19" s="202">
         <v>416.3</v>
       </c>
-      <c r="J19" s="3">
+      <c r="J19" s="202">
         <v>396</v>
       </c>
-      <c r="K19" s="158">
+      <c r="K19" s="219">
         <v>0.25206874602163998</v>
       </c>
-      <c r="L19" s="3">
+      <c r="L19" s="202">
         <v>20</v>
       </c>
-      <c r="M19" s="3">
+      <c r="M19" s="202">
         <v>765</v>
       </c>
-      <c r="N19" s="5">
+      <c r="N19" s="204">
         <v>0.48695098663271003</v>
       </c>
-      <c r="O19" s="3">
+      <c r="O19" s="202">
         <v>237</v>
       </c>
-      <c r="P19" s="3">
+      <c r="P19" s="202">
         <v>160</v>
       </c>
-      <c r="Q19" s="3">
+      <c r="Q19" s="202">
         <v>0</v>
       </c>
-      <c r="R19" s="5">
+      <c r="R19" s="204">
         <v>0.84086569064289995</v>
       </c>
-      <c r="S19" s="3"/>
-      <c r="T19" s="3" t="s">
+      <c r="S19" s="202"/>
+      <c r="T19" s="202" t="s">
         <v>26</v>
       </c>
-      <c r="W19" s="5"/>
-      <c r="Y19" s="3" t="s">
+      <c r="W19" s="204"/>
+      <c r="Y19" s="202" t="s">
         <v>25</v>
       </c>
-      <c r="Z19"/>
+      <c r="Z19" s="201"/>
     </row>
     <row r="20" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
+      <c r="A20" s="202" t="s">
         <v>28</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="B20" s="202" t="s">
         <v>27</v>
       </c>
-      <c r="C20" s="3">
+      <c r="C20" s="202">
         <v>47</v>
       </c>
-      <c r="D20" s="3">
+      <c r="D20" s="202">
         <v>43</v>
       </c>
-      <c r="E20" s="8">
+      <c r="E20" s="203">
         <v>42158</v>
       </c>
-      <c r="F20" s="8">
+      <c r="F20" s="203">
         <v>42249</v>
       </c>
-      <c r="G20" s="3">
+      <c r="G20" s="202">
         <v>1571</v>
       </c>
-      <c r="H20" s="5">
+      <c r="H20" s="204">
         <v>0.26500000000000001</v>
       </c>
-      <c r="I20" s="3">
+      <c r="I20" s="202">
         <v>416.3</v>
       </c>
-      <c r="J20" s="3">
+      <c r="J20" s="202">
         <v>396</v>
       </c>
-      <c r="K20" s="158">
+      <c r="K20" s="219">
         <v>0.25206874602163998</v>
       </c>
-      <c r="L20" s="3">
+      <c r="L20" s="202">
         <v>20</v>
       </c>
-      <c r="M20" s="3">
+      <c r="M20" s="202">
         <v>765</v>
       </c>
-      <c r="N20" s="5">
+      <c r="N20" s="204">
         <v>0.48695098663271003</v>
       </c>
-      <c r="O20" s="3">
+      <c r="O20" s="202">
         <v>237</v>
       </c>
-      <c r="P20" s="3">
+      <c r="P20" s="202">
         <v>160</v>
       </c>
-      <c r="Q20" s="3">
+      <c r="Q20" s="202">
         <v>0</v>
       </c>
-      <c r="R20" s="5">
+      <c r="R20" s="204">
         <v>0.84086569064289995</v>
       </c>
-      <c r="S20" s="3"/>
-      <c r="T20" s="3" t="s">
+      <c r="S20" s="202"/>
+      <c r="T20" s="202" t="s">
         <v>26</v>
       </c>
-      <c r="W20" s="5"/>
-      <c r="Y20" s="3" t="s">
+      <c r="W20" s="204"/>
+      <c r="Y20" s="202" t="s">
         <v>25</v>
       </c>
-      <c r="Z20"/>
+      <c r="Z20" s="201"/>
     </row>
     <row r="21" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
+      <c r="A21" s="202" t="s">
         <v>28</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="B21" s="202" t="s">
         <v>27</v>
       </c>
-      <c r="C21" s="3">
+      <c r="C21" s="202">
         <v>47</v>
       </c>
-      <c r="D21" s="3">
+      <c r="D21" s="202">
         <v>43</v>
       </c>
-      <c r="E21" s="8">
+      <c r="E21" s="203">
         <v>42158</v>
       </c>
-      <c r="F21" s="8">
+      <c r="F21" s="203">
         <v>42249</v>
       </c>
-      <c r="G21" s="3">
+      <c r="G21" s="202">
         <v>1571</v>
       </c>
-      <c r="H21" s="5">
+      <c r="H21" s="204">
         <v>0.26500000000000001</v>
       </c>
-      <c r="I21" s="3">
+      <c r="I21" s="202">
         <v>416.3</v>
       </c>
-      <c r="J21" s="3">
+      <c r="J21" s="202">
         <v>396</v>
       </c>
-      <c r="K21" s="158">
+      <c r="K21" s="219">
         <v>0.25206874602163998</v>
       </c>
-      <c r="L21" s="3">
+      <c r="L21" s="202">
         <v>20</v>
       </c>
-      <c r="M21" s="3">
+      <c r="M21" s="202">
         <v>765</v>
       </c>
-      <c r="N21" s="5">
+      <c r="N21" s="204">
         <v>0.48695098663271003</v>
       </c>
-      <c r="O21" s="3">
+      <c r="O21" s="202">
         <v>237</v>
       </c>
-      <c r="P21" s="3">
+      <c r="P21" s="202">
         <v>160</v>
       </c>
-      <c r="Q21" s="3">
+      <c r="Q21" s="202">
         <v>0</v>
       </c>
-      <c r="R21" s="5">
+      <c r="R21" s="204">
         <v>0.84086569064289995</v>
       </c>
-      <c r="S21" s="3"/>
-      <c r="T21" s="3" t="s">
+      <c r="S21" s="202"/>
+      <c r="T21" s="202" t="s">
         <v>26</v>
       </c>
-      <c r="W21" s="5"/>
-      <c r="Y21" s="3" t="s">
+      <c r="W21" s="204"/>
+      <c r="Y21" s="202" t="s">
         <v>25</v>
       </c>
-      <c r="Z21"/>
+      <c r="Z21" s="201"/>
     </row>
     <row r="22" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A22" s="10" t="s">
+      <c r="A22" s="215" t="s">
         <v>24</v>
       </c>
-      <c r="B22" s="10"/>
-      <c r="C22" s="10"/>
-      <c r="D22" s="10"/>
-      <c r="E22" s="12"/>
-      <c r="F22" s="12"/>
-      <c r="G22" s="10">
+      <c r="B22" s="215"/>
+      <c r="C22" s="215"/>
+      <c r="D22" s="215"/>
+      <c r="E22" s="216"/>
+      <c r="F22" s="216"/>
+      <c r="G22" s="215">
         <v>1571</v>
       </c>
-      <c r="H22" s="11"/>
-      <c r="I22" s="10">
+      <c r="H22" s="220"/>
+      <c r="I22" s="215">
         <v>416.3</v>
       </c>
-      <c r="J22" s="10">
+      <c r="J22" s="215">
         <v>396</v>
       </c>
-      <c r="K22" s="159">
+      <c r="K22" s="221">
         <v>0.25206874602163998</v>
       </c>
-      <c r="L22" s="10">
+      <c r="L22" s="215">
         <v>20</v>
       </c>
-      <c r="M22" s="10">
+      <c r="M22" s="215">
         <v>765</v>
       </c>
-      <c r="N22" s="11">
+      <c r="N22" s="220">
         <v>0.48695098663271003</v>
       </c>
-      <c r="O22" s="10">
+      <c r="O22" s="215">
         <v>237</v>
       </c>
-      <c r="P22" s="10">
+      <c r="P22" s="215">
         <v>160</v>
       </c>
-      <c r="Q22" s="10">
+      <c r="Q22" s="215">
         <v>0</v>
       </c>
-      <c r="R22" s="11">
+      <c r="R22" s="220">
         <v>0.84086569064289995</v>
       </c>
-      <c r="S22" s="10"/>
-      <c r="T22" s="10" t="s">
+      <c r="S22" s="215"/>
+      <c r="T22" s="215" t="s">
         <v>22</v>
       </c>
-      <c r="U22" s="10"/>
-      <c r="V22" s="10"/>
-      <c r="W22" s="11"/>
-      <c r="X22" s="9"/>
-      <c r="Y22" s="9"/>
-      <c r="Z22"/>
+      <c r="U22" s="215"/>
+      <c r="V22" s="215"/>
+      <c r="W22" s="220"/>
+      <c r="X22" s="218"/>
+      <c r="Y22" s="218"/>
+      <c r="Z22" s="201"/>
     </row>
     <row r="23" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A23" s="13" t="s">
+      <c r="A23" s="213" t="s">
         <v>23</v>
       </c>
-      <c r="B23" s="10"/>
-      <c r="C23" s="10"/>
-      <c r="D23" s="10"/>
-      <c r="E23" s="12"/>
-      <c r="F23" s="12"/>
-      <c r="G23" s="10">
+      <c r="B23" s="215"/>
+      <c r="C23" s="215"/>
+      <c r="D23" s="215"/>
+      <c r="E23" s="216"/>
+      <c r="F23" s="216"/>
+      <c r="G23" s="215">
         <v>1571</v>
       </c>
-      <c r="H23" s="11"/>
-      <c r="I23" s="10">
+      <c r="H23" s="220"/>
+      <c r="I23" s="215">
         <v>416.3</v>
       </c>
-      <c r="J23" s="10">
+      <c r="J23" s="215">
         <v>396</v>
       </c>
-      <c r="K23" s="159">
+      <c r="K23" s="221">
         <v>0.25206874602163998</v>
       </c>
-      <c r="L23" s="10">
+      <c r="L23" s="215">
         <v>20</v>
       </c>
-      <c r="M23" s="10">
+      <c r="M23" s="215">
         <v>765</v>
       </c>
-      <c r="N23" s="11">
+      <c r="N23" s="220">
         <v>0.48695098663271003</v>
       </c>
-      <c r="O23" s="10">
+      <c r="O23" s="215">
         <v>237</v>
       </c>
-      <c r="P23" s="10">
+      <c r="P23" s="215">
         <v>160</v>
       </c>
-      <c r="Q23" s="10">
+      <c r="Q23" s="215">
         <v>0</v>
       </c>
-      <c r="R23" s="11">
+      <c r="R23" s="220">
         <v>0.84086569064289995</v>
       </c>
-      <c r="S23" s="10"/>
-      <c r="T23" s="10" t="s">
+      <c r="S23" s="215"/>
+      <c r="T23" s="215" t="s">
         <v>22</v>
       </c>
-      <c r="U23" s="10"/>
-      <c r="V23" s="10"/>
-      <c r="W23" s="11"/>
-      <c r="X23" s="9"/>
-      <c r="Y23" s="9"/>
-      <c r="Z23"/>
+      <c r="U23" s="215"/>
+      <c r="V23" s="215"/>
+      <c r="W23" s="220"/>
+      <c r="X23" s="218"/>
+      <c r="Y23" s="218"/>
+      <c r="Z23" s="201"/>
     </row>
     <row r="24" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="L24" s="3"/>
-      <c r="N24" s="5"/>
-      <c r="O24" s="3"/>
-      <c r="R24" s="5"/>
-      <c r="S24" s="3"/>
-      <c r="W24" s="5"/>
-      <c r="Z24"/>
+      <c r="L24" s="202"/>
+      <c r="N24" s="204"/>
+      <c r="O24" s="202"/>
+      <c r="R24" s="204"/>
+      <c r="S24" s="202"/>
+      <c r="W24" s="204"/>
+      <c r="Z24" s="201"/>
     </row>
     <row r="25" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A25" s="3">
+      <c r="A25" s="202">
         <v>0</v>
       </c>
-      <c r="B25" s="3">
+      <c r="B25" s="202">
         <v>1</v>
       </c>
-      <c r="C25" s="3">
+      <c r="C25" s="202">
         <v>2</v>
       </c>
-      <c r="D25" s="3">
+      <c r="D25" s="202">
         <v>3</v>
       </c>
-      <c r="E25" s="3">
+      <c r="E25" s="202">
         <v>4</v>
       </c>
-      <c r="F25" s="3">
+      <c r="F25" s="202">
         <v>5</v>
       </c>
-      <c r="G25" s="3">
+      <c r="G25" s="202">
         <v>6</v>
       </c>
-      <c r="H25" s="3">
+      <c r="H25" s="202">
         <v>7</v>
       </c>
-      <c r="I25" s="3">
+      <c r="I25" s="202">
         <v>8</v>
       </c>
-      <c r="J25" s="3">
+      <c r="J25" s="202">
         <v>9</v>
       </c>
-      <c r="K25" s="3">
+      <c r="K25" s="202">
         <v>10</v>
       </c>
-      <c r="L25" s="3">
+      <c r="L25" s="202">
         <v>11</v>
       </c>
-      <c r="M25" s="3">
+      <c r="M25" s="202">
         <v>12</v>
       </c>
-      <c r="N25" s="3">
+      <c r="N25" s="202">
         <v>13</v>
       </c>
-      <c r="O25" s="3">
+      <c r="O25" s="202">
         <v>14</v>
       </c>
-      <c r="P25" s="3">
+      <c r="P25" s="202">
         <v>15</v>
       </c>
-      <c r="Q25" s="3">
+      <c r="Q25" s="202">
         <v>16</v>
       </c>
-      <c r="R25" s="3">
+      <c r="R25" s="202">
         <v>17</v>
       </c>
-      <c r="S25" s="3">
+      <c r="S25" s="202">
         <v>18</v>
       </c>
-      <c r="T25" s="3">
+      <c r="T25" s="202">
         <v>19</v>
       </c>
-      <c r="U25" s="3">
+      <c r="U25" s="202">
         <v>20</v>
       </c>
-      <c r="V25" s="3">
+      <c r="V25" s="202">
         <v>21</v>
       </c>
-      <c r="W25" s="3">
+      <c r="W25" s="202">
         <v>22</v>
       </c>
-      <c r="X25" s="3">
+      <c r="X25" s="202">
         <v>23</v>
       </c>
-      <c r="Y25" s="3">
+      <c r="Y25" s="202">
         <v>24</v>
       </c>
     </row>
     <row r="26" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="E26" s="3"/>
-      <c r="F26" s="3"/>
-      <c r="H26" s="3"/>
-      <c r="K26" s="3"/>
-      <c r="L26" s="3"/>
-      <c r="O26" s="3"/>
-      <c r="S26" s="3"/>
+      <c r="E26" s="202"/>
+      <c r="F26" s="202"/>
+      <c r="H26" s="202"/>
+      <c r="K26" s="202"/>
+      <c r="L26" s="202"/>
+      <c r="O26" s="202"/>
+      <c r="S26" s="202"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -8211,7 +8297,7 @@
     <mergeCell ref="A3:AA3"/>
   </mergeCells>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.55118110236220474" bottom="0.55118110236220474" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="9" scale="61" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="60" fitToHeight="0" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>